<commit_message>
Updated the latest status as per SQL
</commit_message>
<xml_diff>
--- a/Excel/Predictive Process Mining/Attributes_Overview.xlsx
+++ b/Excel/Predictive Process Mining/Attributes_Overview.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339F6018-0030-4C1F-A2BA-B9FBBF934D55}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B9F08E-D7ED-439E-A454-149D32C84B6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1524" yWindow="1524" windowWidth="17280" windowHeight="9132" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Case Level Attributes</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Comments for even level</t>
+  </si>
+  <si>
+    <t>handover count per case</t>
+  </si>
+  <si>
+    <t>bit stating whether it is rework or not</t>
+  </si>
+  <si>
+    <t>not included in the event_consolidated</t>
   </si>
 </sst>
 </file>
@@ -425,25 +437,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -453,8 +465,11 @@
       <c r="C2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -464,8 +479,11 @@
       <c r="C3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -475,8 +493,11 @@
       <c r="C4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -486,8 +507,11 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -498,7 +522,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -506,7 +530,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -514,7 +538,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -522,7 +546,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -530,7 +554,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -538,7 +562,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>16</v>
       </c>
@@ -546,7 +570,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -554,7 +578,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -562,7 +586,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -570,7 +594,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -578,7 +602,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
@@ -586,7 +610,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>